<commit_message>
se ven los nombres
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.yeguez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F50E1830-C85A-407B-8F43-BAC7A4D693E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367256BE-1B60-4B97-84E1-C58533823DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{847C556D-73AA-4868-8A87-4F1A7789FCA3}"/>
   </bookViews>
@@ -120,6 +120,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,15 +161,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -515,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC19C62-E257-4EDD-83F5-CB95EF3B0484}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +532,7 @@
     <col min="5" max="5" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -558,11 +562,11 @@
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>45787</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -575,11 +579,12 @@
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>45788</v>
       </c>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -589,14 +594,14 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>45789</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -609,11 +614,11 @@
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>45790</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -626,11 +631,11 @@
       <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>45791</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -640,10 +645,10 @@
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>45792</v>
       </c>
     </row>
@@ -658,5 +663,6 @@
     <hyperlink ref="D7" r:id="rId2" xr:uid="{CB723471-EA0A-4686-B657-5B05CD0DB9C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Envia correo y correcion de nombre de jefatura
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.yeguez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.alexis\Desktop\mvp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367256BE-1B60-4B97-84E1-C58533823DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE811351-2213-4A1F-B2E7-9C86143D6A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{847C556D-73AA-4868-8A87-4F1A7789FCA3}"/>
+    <workbookView xWindow="1810" yWindow="280" windowWidth="14400" windowHeight="10040" xr2:uid="{847C556D-73AA-4868-8A87-4F1A7789FCA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -80,12 +80,6 @@
     <t>JEF-3</t>
   </si>
   <si>
-    <t>Carla Diaz</t>
-  </si>
-  <si>
-    <t>Salvador Rodriguez</t>
-  </si>
-  <si>
     <t>Julieta Sabatinie</t>
   </si>
   <si>
@@ -98,12 +92,6 @@
     <t>Yamilet Perez</t>
   </si>
   <si>
-    <t>carla.diaz@empresa.com</t>
-  </si>
-  <si>
-    <t>salvador.rodriguez@empresa.com</t>
-  </si>
-  <si>
     <t>julieta.sabatinie@empresa.com</t>
   </si>
   <si>
@@ -114,6 +102,18 @@
   </si>
   <si>
     <t xml:space="preserve">yamilet.perez@empresa.com </t>
+  </si>
+  <si>
+    <t>mariavyeguezp@gmail.com</t>
+  </si>
+  <si>
+    <t>Maria Yeguez</t>
+  </si>
+  <si>
+    <t>Rodrigo Gonzalez</t>
+  </si>
+  <si>
+    <t>ro.gonzalezl@duocuc.cl</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -169,8 +169,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,10 +557,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E2" s="4">
         <v>45787</v>
@@ -574,10 +574,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="4">
         <v>45788</v>
@@ -592,10 +592,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4">
         <v>45789</v>
@@ -609,10 +609,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4">
         <v>45790</v>
@@ -626,10 +626,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4">
         <v>45791</v>
@@ -643,10 +643,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>45792</v>
@@ -661,8 +661,10 @@
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{84923F0D-D60B-41E8-94FD-8C87E3AFAA6C}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{CB723471-EA0A-4686-B657-5B05CD0DB9C0}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{A3C16FB7-3B20-4141-AC42-1474B673FFA8}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{F79D90C9-5DB8-47DC-8C9D-873AF768FAF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego la imagen de claro como pie de pagina (banner)
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.alexis\Desktop\mvp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE811351-2213-4A1F-B2E7-9C86143D6A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA93F09D-9268-484A-8648-49A86A81A06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1810" yWindow="280" windowWidth="14400" windowHeight="10040" xr2:uid="{847C556D-73AA-4868-8A87-4F1A7789FCA3}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t xml:space="preserve">yamilet.perez@empresa.com </t>
   </si>
   <si>
-    <t>mariavyeguezp@gmail.com</t>
-  </si>
-  <si>
     <t>Maria Yeguez</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>ro.gonzalezl@duocuc.cl</t>
+  </si>
+  <si>
+    <t>mario.calderons@empresa.com</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,10 +557,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E2" s="4">
         <v>45787</v>
@@ -574,10 +574,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4">
         <v>45788</v>
@@ -661,8 +661,8 @@
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{84923F0D-D60B-41E8-94FD-8C87E3AFAA6C}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{CB723471-EA0A-4686-B657-5B05CD0DB9C0}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{A3C16FB7-3B20-4141-AC42-1474B673FFA8}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{F79D90C9-5DB8-47DC-8C9D-873AF768FAF7}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{F79D90C9-5DB8-47DC-8C9D-873AF768FAF7}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{FF2A049C-15EC-4AAA-B2E5-8103B0B497A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>